<commit_message>
Working on changes with new ids for easier use
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Supporting_Docs/ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Supporting_Docs/ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\Supporting_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4944F-730B-495C-8F58-B11BD065FD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600B7B82-C216-4D55-B055-065A9EF0B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="256">
   <si>
     <t>ID</t>
   </si>
@@ -799,7 +799,13 @@
     <t>How have communities used ERB? Activity selection examples</t>
   </si>
   <si>
-    <t>Background Panel (Considered Steps)</t>
+    <t>Content Panels</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>Project Creation</t>
   </si>
 </sst>
 </file>
@@ -1201,21 +1207,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3400,107 +3402,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" style="78" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="70" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.44140625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="3.21875" style="79" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="70" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="32" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.88671875" style="32" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.109375" style="70" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" style="32" customWidth="1"/>
-    <col min="13" max="13" width="6.5546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" style="70" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.6640625" style="32" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="77.77734375" style="70" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3" style="32" customWidth="1"/>
-    <col min="19" max="19" width="8.5546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="68.77734375" style="70" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.33203125" style="32" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.33203125" style="70" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" style="32" customWidth="1"/>
-    <col min="25" max="25" width="10.77734375" style="79" customWidth="1"/>
-    <col min="26" max="26" width="45.5546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" style="78" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="85" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="32" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" style="78" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="32" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" style="78" customWidth="1"/>
+    <col min="14" max="14" width="45.5546875" style="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
-        <v>93</v>
-      </c>
+    <row r="1" spans="1:14" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="75"/>
       <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="75" t="s">
-        <v>94</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="75"/>
       <c r="E1" s="69" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="75" t="s">
-        <v>95</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F1" s="80"/>
+      <c r="G1" s="83"/>
       <c r="H1" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="75" t="s">
-        <v>96</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="I1" s="80"/>
+      <c r="J1" s="75"/>
       <c r="K1" s="69" t="s">
-        <v>253</v>
-      </c>
-      <c r="L1" s="82"/>
-      <c r="M1" s="75" t="s">
-        <v>97</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="L1" s="80"/>
+      <c r="M1" s="79"/>
       <c r="N1" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="75" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" s="82"/>
-      <c r="S1" s="75" t="s">
-        <v>115</v>
-      </c>
-      <c r="T1" s="69" t="s">
-        <v>90</v>
-      </c>
-      <c r="U1" s="82"/>
-      <c r="V1" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="W1" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="81">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="69" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
         <v>93</v>
       </c>
@@ -3509,62 +3461,34 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="76" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="F2" s="32"/>
-      <c r="G2" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="70" t="s">
-        <v>192</v>
-      </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="77" t="s">
+      <c r="G2" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="71" t="s">
+      <c r="H2" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="76" t="s">
+      <c r="I2" s="67"/>
+      <c r="J2" s="76" t="s">
         <v>101</v>
       </c>
+      <c r="K2" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="32"/>
+      <c r="M2" s="78" t="s">
+        <v>196</v>
+      </c>
       <c r="N2" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q2" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="77" t="s">
-        <v>107</v>
-      </c>
-      <c r="T2" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="32"/>
-      <c r="V2" s="76" t="s">
-        <v>113</v>
-      </c>
-      <c r="W2" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="79" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z2" s="70" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>94</v>
       </c>
@@ -3573,62 +3497,34 @@
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="76" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="F3" s="32"/>
-      <c r="G3" s="76" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="77" t="s">
+      <c r="G3" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="H3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="67"/>
-      <c r="M3" s="76" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="76" t="s">
         <v>102</v>
       </c>
+      <c r="K3" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="32"/>
+      <c r="M3" s="78" t="s">
+        <v>197</v>
+      </c>
       <c r="N3" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q3" s="86" t="s">
-        <v>234</v>
-      </c>
-      <c r="R3" s="32"/>
-      <c r="S3" s="76" t="s">
-        <v>108</v>
-      </c>
-      <c r="T3" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="U3" s="32"/>
-      <c r="V3" s="79" t="s">
-        <v>194</v>
-      </c>
-      <c r="W3" s="70" t="s">
-        <v>195</v>
-      </c>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z3" s="70" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>95</v>
       </c>
@@ -3637,62 +3533,34 @@
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="76" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F4" s="32"/>
-      <c r="G4" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="77" t="s">
+      <c r="G4" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="71" t="s">
+      <c r="H4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="76" t="s">
+      <c r="I4" s="67"/>
+      <c r="J4" s="76" t="s">
         <v>103</v>
       </c>
+      <c r="K4" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="32"/>
+      <c r="M4" s="78" t="s">
+        <v>198</v>
+      </c>
       <c r="N4" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q4" s="86" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="T4" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="W4" s="74" t="s">
-        <v>236</v>
-      </c>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="79" t="s">
-        <v>198</v>
-      </c>
-      <c r="Z4" s="70" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="76" t="s">
         <v>96</v>
       </c>
@@ -3700,55 +3568,35 @@
         <v>69</v>
       </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="70"/>
+      <c r="D5" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>82</v>
+      </c>
       <c r="F5" s="32"/>
-      <c r="G5" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="77" t="s">
+      <c r="G5" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="K5" s="71" t="s">
+      <c r="H5" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="67"/>
-      <c r="M5" s="76" t="s">
+      <c r="I5" s="67"/>
+      <c r="J5" s="76" t="s">
         <v>104</v>
       </c>
+      <c r="K5" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="32"/>
+      <c r="M5" s="78" t="s">
+        <v>202</v>
+      </c>
       <c r="N5" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q5" s="86" t="s">
-        <v>238</v>
-      </c>
-      <c r="R5" s="32"/>
-      <c r="S5" s="87" t="s">
-        <v>110</v>
-      </c>
-      <c r="T5" s="74" t="s">
-        <v>237</v>
-      </c>
-      <c r="U5" s="32"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="79" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z5" s="70" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>97</v>
       </c>
@@ -3756,51 +3604,35 @@
         <v>85</v>
       </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="70"/>
+      <c r="D6" s="78" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>255</v>
+      </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="70"/>
+      <c r="G6" s="84" t="s">
+        <v>247</v>
+      </c>
+      <c r="H6" s="72" t="s">
+        <v>248</v>
+      </c>
       <c r="I6" s="32"/>
-      <c r="J6" s="84" t="s">
-        <v>247</v>
-      </c>
-      <c r="K6" s="72" t="s">
-        <v>248</v>
+      <c r="J6" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="70" t="s">
+        <v>46</v>
       </c>
       <c r="L6" s="32"/>
-      <c r="M6" s="76" t="s">
-        <v>105</v>
+      <c r="M6" s="78" t="s">
+        <v>204</v>
       </c>
       <c r="N6" s="70" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q6" s="86" t="s">
-        <v>241</v>
-      </c>
-      <c r="R6" s="32"/>
-      <c r="S6" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="T6" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="U6" s="32"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="79" t="s">
-        <v>204</v>
-      </c>
-      <c r="Z6" s="70" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="76" t="s">
         <v>114</v>
       </c>
@@ -3808,47 +3640,27 @@
         <v>71</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="79"/>
+      <c r="D7" s="78"/>
       <c r="E7" s="70"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="70"/>
+      <c r="G7" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" s="72" t="s">
+        <v>250</v>
+      </c>
       <c r="I7" s="32"/>
-      <c r="J7" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="K7" s="72" t="s">
-        <v>250</v>
-      </c>
-      <c r="L7" s="32"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="76" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q7" s="86" t="s">
-        <v>242</v>
-      </c>
-      <c r="R7" s="32"/>
-      <c r="S7" s="76" t="s">
-        <v>112</v>
-      </c>
-      <c r="T7" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="U7" s="32"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="70"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="79" t="s">
+      <c r="J7" s="77"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="Z7" s="70" t="s">
+      <c r="N7" s="70" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="76" t="s">
         <v>115</v>
       </c>
@@ -3856,639 +3668,590 @@
         <v>72</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="79"/>
+      <c r="D8" s="78"/>
       <c r="E8" s="70"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="70"/>
+      <c r="G8" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="H8" s="72" t="s">
+        <v>252</v>
+      </c>
       <c r="I8" s="32"/>
-      <c r="J8" s="79" t="s">
-        <v>251</v>
-      </c>
-      <c r="K8" s="72" t="s">
-        <v>252</v>
-      </c>
+      <c r="J8" s="78"/>
+      <c r="K8" s="70"/>
       <c r="L8" s="32"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q8" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="32"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="79" t="s">
+      <c r="M8" s="78" t="s">
         <v>207</v>
       </c>
-      <c r="Z8" s="70" t="s">
+      <c r="N8" s="70" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="70"/>
+    <row r="9" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="70" t="s">
+        <v>50</v>
+      </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="79"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="70"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="70"/>
+      <c r="G9" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="82" t="s">
+        <v>4</v>
+      </c>
       <c r="I9" s="32"/>
-      <c r="J9" s="79"/>
+      <c r="J9" s="78"/>
       <c r="K9" s="70"/>
       <c r="L9" s="32"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q9" s="86" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="32"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="79"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="79" t="s">
+      <c r="M9" s="78" t="s">
         <v>208</v>
       </c>
-      <c r="Z9" s="70" t="s">
+      <c r="N9" s="70" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
-      <c r="B10" s="70"/>
+    <row r="10" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>51</v>
+      </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="79"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="70"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="70"/>
+      <c r="G10" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="82" t="s">
+        <v>234</v>
+      </c>
       <c r="I10" s="32"/>
-      <c r="J10" s="79"/>
+      <c r="J10" s="78"/>
       <c r="K10" s="70"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q10" s="86" t="s">
-        <v>243</v>
-      </c>
-      <c r="R10" s="32"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="70"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="79" t="s">
+      <c r="M10" s="78" t="s">
         <v>209</v>
       </c>
-      <c r="Z10" s="70" t="s">
+      <c r="N10" s="70" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="79"/>
-      <c r="B11" s="70"/>
+    <row r="11" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>52</v>
+      </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="79"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="70"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="70"/>
+      <c r="G11" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="82" t="s">
+        <v>36</v>
+      </c>
       <c r="I11" s="32"/>
-      <c r="J11" s="79"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="70"/>
       <c r="L11" s="32"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q11" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="R11" s="32"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="70"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="79"/>
-      <c r="W11" s="70"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="79" t="s">
+      <c r="M11" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="Z11" s="70" t="s">
+      <c r="N11" s="70" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
+    <row r="12" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="78"/>
       <c r="B12" s="70"/>
       <c r="C12" s="32"/>
-      <c r="D12" s="79"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="70"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="70"/>
+      <c r="G12" s="85" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="82" t="s">
+        <v>238</v>
+      </c>
       <c r="I12" s="32"/>
-      <c r="J12" s="79"/>
+      <c r="J12" s="78"/>
       <c r="K12" s="70"/>
       <c r="L12" s="32"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="76" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q12" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="R12" s="32"/>
-      <c r="S12" s="79"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="79"/>
-      <c r="W12" s="70"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="79" t="s">
+      <c r="M12" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="Z12" s="70" t="s">
+      <c r="N12" s="70" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+    <row r="13" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="78"/>
       <c r="B13" s="70"/>
       <c r="C13" s="32"/>
-      <c r="D13" s="79"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="70"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="70"/>
+      <c r="G13" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="82" t="s">
+        <v>241</v>
+      </c>
       <c r="I13" s="32"/>
-      <c r="J13" s="79"/>
+      <c r="J13" s="78"/>
       <c r="K13" s="70"/>
       <c r="L13" s="32"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q13" s="70" t="s">
-        <v>12</v>
-      </c>
-      <c r="R13" s="32"/>
-      <c r="S13" s="79"/>
-      <c r="T13" s="70"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="70"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="79" t="s">
+      <c r="M13" s="78" t="s">
         <v>219</v>
       </c>
-      <c r="Z13" s="70" t="s">
+      <c r="N13" s="70" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+    <row r="14" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="78"/>
       <c r="B14" s="70"/>
       <c r="C14" s="32"/>
-      <c r="D14" s="79"/>
+      <c r="D14" s="78"/>
       <c r="E14" s="70"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="70"/>
+      <c r="G14" s="85" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="82" t="s">
+        <v>242</v>
+      </c>
       <c r="I14" s="32"/>
-      <c r="J14" s="79"/>
+      <c r="J14" s="78"/>
       <c r="K14" s="70"/>
       <c r="L14" s="32"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="76" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q14" s="70" t="s">
-        <v>13</v>
-      </c>
-      <c r="R14" s="32"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="79" t="s">
+      <c r="M14" s="78" t="s">
         <v>221</v>
       </c>
-      <c r="Z14" s="70" t="s">
+      <c r="N14" s="70" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="79"/>
+    <row r="15" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="78"/>
       <c r="B15" s="70"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="79"/>
+      <c r="D15" s="78"/>
       <c r="E15" s="70"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="70"/>
+      <c r="G15" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="82" t="s">
+        <v>20</v>
+      </c>
       <c r="I15" s="32"/>
-      <c r="J15" s="79"/>
+      <c r="J15" s="78"/>
       <c r="K15" s="70"/>
       <c r="L15" s="32"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q15" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="70"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="79" t="s">
+      <c r="M15" s="78" t="s">
         <v>224</v>
       </c>
-      <c r="Z15" s="70" t="s">
+      <c r="N15" s="70" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="79"/>
+    <row r="16" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="78"/>
       <c r="B16" s="70"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="79"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="70"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="70"/>
+      <c r="G16" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="82" t="s">
+        <v>21</v>
+      </c>
       <c r="I16" s="32"/>
-      <c r="J16" s="79"/>
+      <c r="J16" s="78"/>
       <c r="K16" s="70"/>
       <c r="L16" s="32"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q16" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="32"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="70"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="79"/>
-      <c r="W16" s="70"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="79" t="s">
+      <c r="M16" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="Z16" s="70" t="s">
+      <c r="N16" s="70" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
+    <row r="17" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="78"/>
       <c r="B17" s="70"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="79"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="70"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="70"/>
+      <c r="G17" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="82" t="s">
+        <v>243</v>
+      </c>
       <c r="I17" s="32"/>
-      <c r="J17" s="79"/>
+      <c r="J17" s="78"/>
       <c r="K17" s="70"/>
       <c r="L17" s="32"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q17" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="R17" s="32"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="79"/>
-      <c r="W17" s="70"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="79" t="s">
+      <c r="M17" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="Z17" s="70" t="s">
+      <c r="N17" s="70" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
+    <row r="18" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="78"/>
       <c r="B18" s="70"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="79"/>
+      <c r="D18" s="78"/>
       <c r="E18" s="70"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="70"/>
+      <c r="G18" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="70" t="s">
+        <v>38</v>
+      </c>
       <c r="I18" s="32"/>
-      <c r="J18" s="79"/>
+      <c r="J18" s="78"/>
       <c r="K18" s="70"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q18" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="R18" s="32"/>
-      <c r="S18" s="79"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="79"/>
-      <c r="W18" s="70"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="79" t="s">
+      <c r="M18" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="Z18" s="70" t="s">
+      <c r="N18" s="70" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="79"/>
+    <row r="19" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="78"/>
       <c r="B19" s="70"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="79"/>
+      <c r="D19" s="76"/>
       <c r="E19" s="70"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="70"/>
+      <c r="G19" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>39</v>
+      </c>
       <c r="I19" s="32"/>
-      <c r="J19" s="79"/>
+      <c r="J19" s="78"/>
       <c r="K19" s="70"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="70"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="76" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q19" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="R19" s="32"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="79"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="78"/>
-      <c r="Z19" s="73"/>
-    </row>
-    <row r="20" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="73"/>
+    </row>
+    <row r="20" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="78"/>
       <c r="B20" s="70"/>
       <c r="C20" s="32"/>
-      <c r="D20" s="79"/>
+      <c r="D20" s="76"/>
       <c r="E20" s="70"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="70"/>
+      <c r="G20" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>12</v>
+      </c>
       <c r="I20" s="32"/>
-      <c r="J20" s="79"/>
+      <c r="J20" s="78"/>
       <c r="K20" s="70"/>
       <c r="L20" s="32"/>
-      <c r="M20" s="79"/>
+      <c r="M20" s="78"/>
       <c r="N20" s="70"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q20" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="79"/>
-      <c r="W20" s="70"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="79"/>
-      <c r="Z20" s="70"/>
-    </row>
-    <row r="21" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+    </row>
+    <row r="21" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="78"/>
       <c r="B21" s="70"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="79"/>
+      <c r="D21" s="76"/>
       <c r="E21" s="70"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="70"/>
+      <c r="G21" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>13</v>
+      </c>
       <c r="I21" s="32"/>
-      <c r="J21" s="79"/>
+      <c r="J21" s="78"/>
       <c r="K21" s="70"/>
       <c r="L21" s="32"/>
-      <c r="M21" s="79"/>
+      <c r="M21" s="78"/>
       <c r="N21" s="70"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="76" t="s">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D22" s="76"/>
+      <c r="G22" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D23" s="76"/>
+      <c r="G23" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D24" s="76"/>
+      <c r="G24" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="76"/>
+      <c r="G25" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D26" s="76"/>
+      <c r="G26" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D27" s="76"/>
+      <c r="G27" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D28" s="76"/>
+      <c r="G28" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="Q21" s="70" t="s">
+      <c r="H28" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="R21" s="32"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="79"/>
-      <c r="W21" s="70"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="79"/>
-      <c r="Z21" s="70"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G22" s="76"/>
-      <c r="P22" s="76" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D29" s="76"/>
+      <c r="G29" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="Q22" s="70" t="s">
+      <c r="H29" s="70" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G23" s="76"/>
-      <c r="P23" s="76" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D30" s="76"/>
+      <c r="G30" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="Q23" s="70" t="s">
+      <c r="H30" s="70" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G24" s="76"/>
-      <c r="P24" s="76" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D31" s="76"/>
+      <c r="G31" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="Q24" s="70" t="s">
+      <c r="H31" s="70" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G25" s="76"/>
-      <c r="P25" s="76" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D32" s="76"/>
+      <c r="G32" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="Q25" s="70" t="s">
+      <c r="H32" s="70" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G26" s="76"/>
-      <c r="P26" s="76" t="s">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D33" s="76"/>
+      <c r="G33" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="Q26" s="70" t="s">
+      <c r="H33" s="70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G27" s="76"/>
-      <c r="P27" s="76" t="s">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D34" s="76"/>
+      <c r="G34" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="Q27" s="70" t="s">
+      <c r="H34" s="70" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G28" s="76"/>
-      <c r="P28" s="76" t="s">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D35" s="76"/>
+      <c r="G35" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="Q28" s="70" t="s">
+      <c r="H35" s="70" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G29" s="76"/>
-      <c r="P29" s="76" t="s">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D36" s="76"/>
+      <c r="G36" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="Q29" s="70" t="s">
+      <c r="H36" s="70" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G30" s="76"/>
-      <c r="P30" s="76" t="s">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D37" s="76"/>
+      <c r="G37" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="Q30" s="70" t="s">
+      <c r="H37" s="70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G31" s="76"/>
-      <c r="P31" s="76" t="s">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D38" s="76"/>
+      <c r="G38" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="Q31" s="86" t="s">
+      <c r="H38" s="82" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="G32" s="76"/>
-      <c r="P32" s="85" t="s">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D39" s="76"/>
+      <c r="G39" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="Q32" s="86" t="s">
+      <c r="H39" s="82" t="s">
         <v>246</v>
       </c>
-      <c r="R32" s="83"/>
-    </row>
-    <row r="33" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G33" s="76"/>
-      <c r="P33" s="79" t="s">
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D40" s="76"/>
+      <c r="G40" s="85" t="s">
         <v>239</v>
       </c>
-      <c r="Q33" s="86" t="s">
+      <c r="H40" s="82" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G34" s="76"/>
-      <c r="P34" s="79" t="s">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D41" s="76"/>
+      <c r="G41" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="Q34" s="86" t="s">
+      <c r="H41" s="82" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G35" s="76"/>
-    </row>
-    <row r="36" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G36" s="76"/>
-    </row>
-    <row r="37" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G37" s="76"/>
-    </row>
-    <row r="38" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G38" s="76"/>
-    </row>
-    <row r="39" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G39" s="76"/>
-    </row>
-    <row r="40" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G40" s="76"/>
-    </row>
-    <row r="41" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G41" s="76"/>
-    </row>
-    <row r="42" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G42" s="76"/>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D42" s="76"/>
+      <c r="G42" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" s="72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G43" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G44" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="H44" s="70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G45" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" s="74" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G46" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="H46" s="70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G47" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="H47" s="70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G48" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="H48" s="70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G49" s="85" t="s">
+        <v>194</v>
+      </c>
+      <c r="H49" s="70" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G50" s="87" t="s">
+        <v>235</v>
+      </c>
+      <c r="H50" s="74" t="s">
+        <v>236</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Working on changes with new ids for easier use"
This reverts commit 5e52bdf4fd2e48584f138f2f91c7702c77b1ead7.
</commit_message>
<xml_diff>
--- a/erb_supporting_docs/Code_Resources/ERB/Static_Data/Supporting_Docs/ID_Chart.xlsx
+++ b/erb_supporting_docs/Code_Resources/ERB/Static_Data/Supporting_Docs/ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb_supporting_docs\Code_Resources\ERB\Static_Data\Supporting_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600B7B82-C216-4D55-B055-065A9EF0B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4944F-730B-495C-8F58-B11BD065FD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="254">
   <si>
     <t>ID</t>
   </si>
@@ -799,13 +799,7 @@
     <t>How have communities used ERB? Activity selection examples</t>
   </si>
   <si>
-    <t>Content Panels</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>Project Creation</t>
+    <t>Background Panel (Considered Steps)</t>
   </si>
 </sst>
 </file>
@@ -1207,17 +1201,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3402,57 +3400,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.21875" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" style="70" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.44140625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" style="78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="32" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="85" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.77734375" style="70" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="32" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" style="78" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" style="70" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="32" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" style="78" customWidth="1"/>
-    <col min="14" max="14" width="45.5546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.21875" style="79" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="32" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.88671875" style="32" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.109375" style="70" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="32" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" style="70" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.6640625" style="32" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="77.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3" style="32" customWidth="1"/>
+    <col min="19" max="19" width="8.5546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="68.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.33203125" style="32" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="79" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.33203125" style="70" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" style="32" customWidth="1"/>
+    <col min="25" max="25" width="10.77734375" style="79" customWidth="1"/>
+    <col min="26" max="26" width="45.5546875" style="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75"/>
+    <row r="1" spans="1:26" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="75" t="s">
+        <v>93</v>
+      </c>
       <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="82"/>
+      <c r="D1" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="69" t="s">
+      <c r="F1" s="82"/>
+      <c r="G1" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="69" t="s">
+      <c r="I1" s="82"/>
+      <c r="J1" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="69" t="s">
         <v>253</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="69" t="s">
+      <c r="L1" s="82"/>
+      <c r="M1" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="80"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="69" t="s">
+      <c r="O1" s="82"/>
+      <c r="P1" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="82"/>
+      <c r="S1" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" s="82"/>
+      <c r="V1" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="W1" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="81">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="69" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
         <v>93</v>
       </c>
@@ -3461,34 +3509,62 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="H2" s="70" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="84" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="K2" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="76" t="s">
+      <c r="L2" s="67"/>
+      <c r="M2" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="N2" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="78" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="32"/>
+      <c r="S2" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="T2" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="32"/>
+      <c r="V2" s="76" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="N2" s="70" t="s">
+      <c r="Z2" s="70" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>94</v>
       </c>
@@ -3497,34 +3573,62 @@
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="H3" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="84" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="K3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="76" t="s">
+      <c r="L3" s="67"/>
+      <c r="M3" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="N3" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="78" t="s">
+      <c r="O3" s="32"/>
+      <c r="P3" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="86" t="s">
+        <v>234</v>
+      </c>
+      <c r="R3" s="32"/>
+      <c r="S3" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="32"/>
+      <c r="V3" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="N3" s="70" t="s">
+      <c r="Z3" s="70" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>95</v>
       </c>
@@ -3533,34 +3637,62 @@
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="H4" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="84" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="71" t="s">
+      <c r="K4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="76" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="K4" s="70" t="s">
+      <c r="N4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="78" t="s">
+      <c r="O4" s="32"/>
+      <c r="P4" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="T4" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="32"/>
+      <c r="V4" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="W4" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="79" t="s">
         <v>198</v>
       </c>
-      <c r="N4" s="70" t="s">
+      <c r="Z4" s="70" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="76" t="s">
         <v>96</v>
       </c>
@@ -3568,35 +3700,55 @@
         <v>69</v>
       </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="79"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="H5" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="84" t="s">
+      <c r="I5" s="32"/>
+      <c r="J5" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="71" t="s">
+      <c r="K5" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="76" t="s">
+      <c r="L5" s="67"/>
+      <c r="M5" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="70" t="s">
+      <c r="N5" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="78" t="s">
+      <c r="O5" s="32"/>
+      <c r="P5" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="86" t="s">
+        <v>238</v>
+      </c>
+      <c r="R5" s="32"/>
+      <c r="S5" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" s="74" t="s">
+        <v>237</v>
+      </c>
+      <c r="U5" s="32"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="73"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="N5" s="70" t="s">
+      <c r="Z5" s="70" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="76" t="s">
         <v>97</v>
       </c>
@@ -3604,35 +3756,51 @@
         <v>85</v>
       </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="78" t="s">
-        <v>254</v>
-      </c>
-      <c r="E6" s="70" t="s">
-        <v>255</v>
-      </c>
+      <c r="D6" s="79"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="32"/>
-      <c r="G6" s="84" t="s">
+      <c r="G6" s="79"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="84" t="s">
         <v>247</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="K6" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="76" t="s">
+      <c r="L6" s="32"/>
+      <c r="M6" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="70" t="s">
+      <c r="N6" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="32"/>
-      <c r="M6" s="78" t="s">
+      <c r="O6" s="32"/>
+      <c r="P6" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q6" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="R6" s="32"/>
+      <c r="S6" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="T6" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="32"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="70"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="79" t="s">
         <v>204</v>
       </c>
-      <c r="N6" s="70" t="s">
+      <c r="Z6" s="70" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="76" t="s">
         <v>114</v>
       </c>
@@ -3640,27 +3808,47 @@
         <v>71</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="78"/>
+      <c r="D7" s="79"/>
       <c r="E7" s="70"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="79"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="79" t="s">
         <v>249</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="K7" s="72" t="s">
         <v>250</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="78" t="s">
+      <c r="L7" s="32"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" s="86" t="s">
+        <v>242</v>
+      </c>
+      <c r="R7" s="32"/>
+      <c r="S7" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="T7" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="32"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="79" t="s">
         <v>206</v>
       </c>
-      <c r="N7" s="70" t="s">
+      <c r="Z7" s="70" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="76" t="s">
         <v>115</v>
       </c>
@@ -3668,590 +3856,639 @@
         <v>72</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="78"/>
+      <c r="D8" s="79"/>
       <c r="E8" s="70"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="79"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="79" t="s">
         <v>251</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="K8" s="72" t="s">
         <v>252</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="70"/>
       <c r="L8" s="32"/>
-      <c r="M8" s="78" t="s">
+      <c r="M8" s="79"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q8" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="32"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="79" t="s">
         <v>207</v>
       </c>
-      <c r="N8" s="70" t="s">
+      <c r="Z8" s="70" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>50</v>
-      </c>
+    <row r="9" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="79"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="32"/>
-      <c r="D9" s="78"/>
+      <c r="D9" s="79"/>
       <c r="E9" s="70"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="85" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="82" t="s">
-        <v>4</v>
-      </c>
+      <c r="G9" s="79"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="32"/>
-      <c r="J9" s="78"/>
+      <c r="J9" s="79"/>
       <c r="K9" s="70"/>
       <c r="L9" s="32"/>
-      <c r="M9" s="78" t="s">
+      <c r="M9" s="79"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="32"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="79" t="s">
         <v>208</v>
       </c>
-      <c r="N9" s="70" t="s">
+      <c r="Z9" s="70" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>51</v>
-      </c>
+    <row r="10" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="79"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="32"/>
-      <c r="D10" s="78"/>
+      <c r="D10" s="79"/>
       <c r="E10" s="70"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="82" t="s">
-        <v>234</v>
-      </c>
+      <c r="G10" s="79"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="32"/>
-      <c r="J10" s="78"/>
+      <c r="J10" s="79"/>
       <c r="K10" s="70"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="78" t="s">
+      <c r="M10" s="79"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="76" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q10" s="86" t="s">
+        <v>243</v>
+      </c>
+      <c r="R10" s="32"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="70"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="79" t="s">
         <v>209</v>
       </c>
-      <c r="N10" s="70" t="s">
+      <c r="Z10" s="70" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="70" t="s">
-        <v>52</v>
-      </c>
+    <row r="11" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="79"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="32"/>
-      <c r="D11" s="78"/>
+      <c r="D11" s="79"/>
       <c r="E11" s="70"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="82" t="s">
-        <v>36</v>
-      </c>
+      <c r="G11" s="79"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="78"/>
+      <c r="J11" s="79"/>
       <c r="K11" s="70"/>
       <c r="L11" s="32"/>
-      <c r="M11" s="78" t="s">
+      <c r="M11" s="79"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="76" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q11" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="32"/>
+      <c r="S11" s="79"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="79"/>
+      <c r="W11" s="70"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="N11" s="70" t="s">
+      <c r="Z11" s="70" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+    <row r="12" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="79"/>
       <c r="B12" s="70"/>
       <c r="C12" s="32"/>
-      <c r="D12" s="78"/>
+      <c r="D12" s="79"/>
       <c r="E12" s="70"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="85" t="s">
-        <v>120</v>
-      </c>
-      <c r="H12" s="82" t="s">
-        <v>238</v>
-      </c>
+      <c r="G12" s="79"/>
+      <c r="H12" s="70"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="78"/>
+      <c r="J12" s="79"/>
       <c r="K12" s="70"/>
       <c r="L12" s="32"/>
-      <c r="M12" s="78" t="s">
+      <c r="M12" s="79"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q12" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12" s="32"/>
+      <c r="S12" s="79"/>
+      <c r="T12" s="70"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="70"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="79" t="s">
         <v>216</v>
       </c>
-      <c r="N12" s="70" t="s">
+      <c r="Z12" s="70" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+    <row r="13" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="79"/>
       <c r="B13" s="70"/>
       <c r="C13" s="32"/>
-      <c r="D13" s="78"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="70"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="85" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="82" t="s">
-        <v>241</v>
-      </c>
+      <c r="G13" s="79"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="32"/>
-      <c r="J13" s="78"/>
+      <c r="J13" s="79"/>
       <c r="K13" s="70"/>
       <c r="L13" s="32"/>
-      <c r="M13" s="78" t="s">
+      <c r="M13" s="79"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q13" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="32"/>
+      <c r="S13" s="79"/>
+      <c r="T13" s="70"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="79"/>
+      <c r="W13" s="70"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="N13" s="70" t="s">
+      <c r="Z13" s="70" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78"/>
+    <row r="14" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="79"/>
       <c r="B14" s="70"/>
       <c r="C14" s="32"/>
-      <c r="D14" s="78"/>
+      <c r="D14" s="79"/>
       <c r="E14" s="70"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="85" t="s">
-        <v>122</v>
-      </c>
-      <c r="H14" s="82" t="s">
-        <v>242</v>
-      </c>
+      <c r="G14" s="79"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="78"/>
+      <c r="J14" s="79"/>
       <c r="K14" s="70"/>
       <c r="L14" s="32"/>
-      <c r="M14" s="78" t="s">
+      <c r="M14" s="79"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q14" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" s="32"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="70"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="70"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="79" t="s">
         <v>221</v>
       </c>
-      <c r="N14" s="70" t="s">
+      <c r="Z14" s="70" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
+    <row r="15" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="79"/>
       <c r="B15" s="70"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="78"/>
+      <c r="D15" s="79"/>
       <c r="E15" s="70"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="H15" s="82" t="s">
-        <v>20</v>
-      </c>
+      <c r="G15" s="79"/>
+      <c r="H15" s="70"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="78"/>
+      <c r="J15" s="79"/>
       <c r="K15" s="70"/>
       <c r="L15" s="32"/>
-      <c r="M15" s="78" t="s">
+      <c r="M15" s="79"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q15" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="R15" s="32"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="70"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="79" t="s">
         <v>224</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="Z15" s="70" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="78"/>
+    <row r="16" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="79"/>
       <c r="B16" s="70"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="78"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="70"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="85" t="s">
-        <v>124</v>
-      </c>
-      <c r="H16" s="82" t="s">
-        <v>21</v>
-      </c>
+      <c r="G16" s="79"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="32"/>
-      <c r="J16" s="78"/>
+      <c r="J16" s="79"/>
       <c r="K16" s="70"/>
       <c r="L16" s="32"/>
-      <c r="M16" s="78" t="s">
+      <c r="M16" s="79"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q16" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="32"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="79"/>
+      <c r="W16" s="70"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="79" t="s">
         <v>226</v>
       </c>
-      <c r="N16" s="70" t="s">
+      <c r="Z16" s="70" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="78"/>
+    <row r="17" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="79"/>
       <c r="B17" s="70"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="78"/>
+      <c r="D17" s="79"/>
       <c r="E17" s="70"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="85" t="s">
-        <v>125</v>
-      </c>
-      <c r="H17" s="82" t="s">
-        <v>243</v>
-      </c>
+      <c r="G17" s="79"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="32"/>
-      <c r="J17" s="78"/>
+      <c r="J17" s="79"/>
       <c r="K17" s="70"/>
       <c r="L17" s="32"/>
-      <c r="M17" s="78" t="s">
+      <c r="M17" s="79"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" s="32"/>
+      <c r="S17" s="79"/>
+      <c r="T17" s="70"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="79"/>
+      <c r="W17" s="70"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="79" t="s">
         <v>228</v>
       </c>
-      <c r="N17" s="70" t="s">
+      <c r="Z17" s="70" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="78"/>
+    <row r="18" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="79"/>
       <c r="B18" s="70"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="78"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="70"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="85" t="s">
-        <v>126</v>
-      </c>
-      <c r="H18" s="70" t="s">
-        <v>38</v>
-      </c>
+      <c r="G18" s="79"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="78"/>
+      <c r="J18" s="79"/>
       <c r="K18" s="70"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="78" t="s">
+      <c r="M18" s="79"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q18" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="R18" s="32"/>
+      <c r="S18" s="79"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="79"/>
+      <c r="W18" s="70"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="79" t="s">
         <v>230</v>
       </c>
-      <c r="N18" s="70" t="s">
+      <c r="Z18" s="70" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="78"/>
+    <row r="19" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="79"/>
       <c r="B19" s="70"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="76"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="70"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="85" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="70" t="s">
-        <v>39</v>
-      </c>
+      <c r="G19" s="76"/>
+      <c r="H19" s="70"/>
       <c r="I19" s="32"/>
-      <c r="J19" s="78"/>
+      <c r="J19" s="79"/>
       <c r="K19" s="70"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="73"/>
-    </row>
-    <row r="20" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q19" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" s="32"/>
+      <c r="S19" s="79"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="79"/>
+      <c r="W19" s="70"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="78"/>
+      <c r="Z19" s="73"/>
+    </row>
+    <row r="20" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="79"/>
       <c r="B20" s="70"/>
       <c r="C20" s="32"/>
-      <c r="D20" s="76"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="70"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="85" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="70" t="s">
-        <v>12</v>
-      </c>
+      <c r="G20" s="76"/>
+      <c r="H20" s="70"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="78"/>
+      <c r="J20" s="79"/>
       <c r="K20" s="70"/>
       <c r="L20" s="32"/>
-      <c r="M20" s="78"/>
+      <c r="M20" s="79"/>
       <c r="N20" s="70"/>
-    </row>
-    <row r="21" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q20" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="R20" s="32"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="79"/>
+      <c r="W20" s="70"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="79"/>
+      <c r="Z20" s="70"/>
+    </row>
+    <row r="21" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="79"/>
       <c r="B21" s="70"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="76"/>
+      <c r="D21" s="79"/>
       <c r="E21" s="70"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="85" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="70" t="s">
-        <v>13</v>
-      </c>
+      <c r="G21" s="76"/>
+      <c r="H21" s="70"/>
       <c r="I21" s="32"/>
-      <c r="J21" s="78"/>
+      <c r="J21" s="79"/>
       <c r="K21" s="70"/>
       <c r="L21" s="32"/>
-      <c r="M21" s="78"/>
+      <c r="M21" s="79"/>
       <c r="N21" s="70"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D22" s="76"/>
-      <c r="G22" s="85" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="70" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D23" s="76"/>
-      <c r="G23" s="85" t="s">
-        <v>131</v>
-      </c>
-      <c r="H23" s="70" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D24" s="76"/>
-      <c r="G24" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="70" t="s">
+      <c r="O21" s="32"/>
+      <c r="P21" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q21" s="70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D25" s="76"/>
-      <c r="G25" s="85" t="s">
-        <v>133</v>
-      </c>
-      <c r="H25" s="70" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D26" s="76"/>
-      <c r="G26" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" s="70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D27" s="76"/>
-      <c r="G27" s="85" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D28" s="76"/>
-      <c r="G28" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="H28" s="70" t="s">
+      <c r="R21" s="32"/>
+      <c r="S21" s="79"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="79"/>
+      <c r="W21" s="70"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="79"/>
+      <c r="Z21" s="70"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G22" s="76"/>
+      <c r="P22" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q22" s="70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G23" s="76"/>
+      <c r="P23" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q23" s="70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G24" s="76"/>
+      <c r="P24" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q24" s="70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G25" s="76"/>
+      <c r="P25" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q25" s="70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G26" s="76"/>
+      <c r="P26" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q26" s="70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G27" s="76"/>
+      <c r="P27" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q27" s="70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G28" s="76"/>
+      <c r="P28" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q28" s="70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G29" s="76"/>
+      <c r="P29" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q29" s="70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G30" s="76"/>
+      <c r="P30" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q30" s="70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D29" s="76"/>
-      <c r="G29" s="85" t="s">
-        <v>137</v>
-      </c>
-      <c r="H29" s="70" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D30" s="76"/>
-      <c r="G30" s="85" t="s">
-        <v>138</v>
-      </c>
-      <c r="H30" s="70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D31" s="76"/>
-      <c r="G31" s="85" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="70" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D32" s="76"/>
-      <c r="G32" s="85" t="s">
-        <v>140</v>
-      </c>
-      <c r="H32" s="70" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D33" s="76"/>
-      <c r="G33" s="85" t="s">
-        <v>141</v>
-      </c>
-      <c r="H33" s="70" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D34" s="76"/>
-      <c r="G34" s="85" t="s">
-        <v>142</v>
-      </c>
-      <c r="H34" s="70" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D35" s="76"/>
-      <c r="G35" s="85" t="s">
-        <v>143</v>
-      </c>
-      <c r="H35" s="70" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D36" s="76"/>
-      <c r="G36" s="85" t="s">
-        <v>144</v>
-      </c>
-      <c r="H36" s="70" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D37" s="76"/>
-      <c r="G37" s="85" t="s">
-        <v>145</v>
-      </c>
-      <c r="H37" s="70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D38" s="76"/>
-      <c r="G38" s="85" t="s">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G31" s="76"/>
+      <c r="P31" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="H38" s="82" t="s">
+      <c r="Q31" s="86" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D39" s="76"/>
-      <c r="G39" s="86" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="G32" s="76"/>
+      <c r="P32" s="85" t="s">
         <v>232</v>
       </c>
-      <c r="H39" s="82" t="s">
+      <c r="Q32" s="86" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D40" s="76"/>
-      <c r="G40" s="85" t="s">
+      <c r="R32" s="83"/>
+    </row>
+    <row r="33" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G33" s="76"/>
+      <c r="P33" s="79" t="s">
         <v>239</v>
       </c>
-      <c r="H40" s="82" t="s">
+      <c r="Q33" s="86" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D41" s="76"/>
-      <c r="G41" s="85" t="s">
+    <row r="34" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G34" s="76"/>
+      <c r="P34" s="79" t="s">
         <v>244</v>
       </c>
-      <c r="H41" s="82" t="s">
+      <c r="Q34" s="86" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D42" s="76"/>
-      <c r="G42" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="H42" s="72" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G43" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" s="70" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G44" s="85" t="s">
-        <v>109</v>
-      </c>
-      <c r="H44" s="70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G45" s="87" t="s">
-        <v>110</v>
-      </c>
-      <c r="H45" s="74" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G46" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="H46" s="70" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G47" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H47" s="70" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G48" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="H48" s="70" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G49" s="85" t="s">
-        <v>194</v>
-      </c>
-      <c r="H49" s="70" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G50" s="87" t="s">
-        <v>235</v>
-      </c>
-      <c r="H50" s="74" t="s">
-        <v>236</v>
-      </c>
+    <row r="35" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G35" s="76"/>
+    </row>
+    <row r="36" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G36" s="76"/>
+    </row>
+    <row r="37" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G37" s="76"/>
+    </row>
+    <row r="38" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G38" s="76"/>
+    </row>
+    <row r="39" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G39" s="76"/>
+    </row>
+    <row r="40" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G40" s="76"/>
+    </row>
+    <row r="41" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G41" s="76"/>
+    </row>
+    <row r="42" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G42" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>